<commit_message>
button on CAN implemented
</commit_message>
<xml_diff>
--- a/perforance_monitoring/tests.xlsx
+++ b/perforance_monitoring/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylve\OneDrive\Bureau\Telemetry-for-the-Formula-Student\perforance_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6528F37-BDBA-41DF-9C40-1DAB10B7E625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889CA6B9-120E-41B1-BDF5-0104CCBC7762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Base system</t>
   </si>
@@ -125,15 +125,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +414,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,6 +532,9 @@
       <c r="E8" s="1">
         <v>200</v>
       </c>
+      <c r="F8" s="1">
+        <v>300</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -552,39 +552,48 @@
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
+      <c r="B11" s="1">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1">
-        <v>30</v>
-      </c>
-      <c r="D12" s="1">
-        <v>30</v>
-      </c>
-      <c r="E12" s="1">
-        <v>30</v>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>